<commit_message>
- Cập nhật các file mẫu import excel. - Sửa lỗi không hiển thị danh sách sinh viên đã đăng ký sự kiện. - Thêm má sự kiện vào dòng nhật kí import sv hoặc cb tham dự (admin debug)
</commit_message>
<xml_diff>
--- a/Sources/DD_RFID/public/download/Mẫu import cán bộ.xlsx
+++ b/Sources/DD_RFID/public/download/Mẫu import cán bộ.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -12,8 +12,8 @@
     <sheet name="data" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="BOMON">data!$B$2:$B$700</definedName>
-    <definedName name="KHOA">data!$A$2:$A$50</definedName>
+    <definedName name="BOMON">data!$B$2:$B$7</definedName>
+    <definedName name="KHOA">data!$A$2:$A$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -536,7 +536,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -599,7 +605,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -662,7 +674,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -725,7 +743,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Down Arrow 4"/>
+        <xdr:cNvPr id="5" name="Down Arrow 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -787,7 +811,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 6"/>
+        <xdr:cNvPr id="6" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2394,7 +2424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>